<commit_message>
21 09 09 home
</commit_message>
<xml_diff>
--- a/코테 벌금표.xlsx
+++ b/코테 벌금표.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\김세준\mine\공부\스터디\코테\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\김세준\스터디\코테\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694E57CD-7592-4A57-8112-94584BA8ADDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F97110C-0B5A-4915-9AAD-1FCC7DC97005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{C09DD02A-E73D-4962-85A2-A63E1B446112}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>오수진</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,10 +73,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>09 06 (월)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2021 백준 코테</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -113,26 +109,29 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Party Money</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09 08 (수)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>○</t>
-  </si>
-  <si>
-    <t>○</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>△</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Party Money</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/asdfrv20/Three_Dorks</t>
+  </si>
+  <si>
+    <t>https://github.com/mercedes6115/test1</t>
+  </si>
+  <si>
+    <t>https://github.com/intlabSeJun/coding_test.git</t>
   </si>
 </sst>
 </file>
@@ -142,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +173,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -183,7 +191,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -470,16 +478,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -546,6 +568,15 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,10 +616,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -901,7 +939,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1C059C-E3B1-40C1-9CB8-8933CD9F208B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:B2"/>
@@ -918,30 +956,30 @@
     <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
+    </row>
+    <row r="2" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>5</v>
@@ -959,64 +997,77 @@
         <v>8</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="25" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="28" t="s">
+        <v>19</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>24</v>
+      <c r="C3" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="16"/>
       <c r="I3" s="17"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="26"/>
-      <c r="B4" s="6" t="s">
+      <c r="J3" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="29"/>
+      <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="8"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="6"/>
       <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="27"/>
+      <c r="J4" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="30"/>
       <c r="B5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>24</v>
+      <c r="C5" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
+      <c r="E5" s="15">
+        <v>3</v>
+      </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="14"/>
       <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="31"/>
+      <c r="J5" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="34"/>
       <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="C6" s="10"/>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
@@ -1024,14 +1075,12 @@
       <c r="H6" s="9"/>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="23"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="26"/>
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="8"/>
       <c r="E7" s="5"/>
       <c r="F7" s="4"/>
@@ -1039,14 +1088,12 @@
       <c r="H7" s="6"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="23"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="26"/>
       <c r="B8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="8"/>
       <c r="E8" s="5"/>
       <c r="F8" s="4"/>
@@ -1054,14 +1101,12 @@
       <c r="H8" s="6"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="23"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="26"/>
       <c r="B9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>22</v>
-      </c>
+      <c r="C9" s="19"/>
       <c r="D9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
@@ -1069,14 +1114,12 @@
       <c r="H9" s="6"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="23"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="26"/>
       <c r="B10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
@@ -1084,14 +1127,12 @@
       <c r="H10" s="6"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="23"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="26"/>
       <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="C11" s="5"/>
       <c r="D11" s="8"/>
       <c r="E11" s="5"/>
       <c r="F11" s="4"/>
@@ -1099,14 +1140,12 @@
       <c r="H11" s="6"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="23"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="26"/>
       <c r="B12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="8"/>
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
@@ -1114,8 +1153,8 @@
       <c r="H12" s="6"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="23"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="26"/>
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1127,14 +1166,12 @@
       <c r="H13" s="6"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="23"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="26"/>
       <c r="B14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="C14" s="5"/>
       <c r="D14" s="8"/>
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
@@ -1142,8 +1179,8 @@
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="23"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="26"/>
       <c r="B15" s="6" t="s">
         <v>0</v>
       </c>
@@ -1155,8 +1192,8 @@
       <c r="H15" s="6"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="23"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="26"/>
       <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
@@ -1169,7 +1206,7 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="23"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="6" t="s">
         <v>2</v>
       </c>
@@ -1193,53 +1230,62 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{5257A6C0-D6E6-42A7-8B6D-F54B9DC5DB2F}"/>
+    <hyperlink ref="J4" r:id="rId2" xr:uid="{F53BEC05-CA13-4E4C-94B8-C10D9B6C73D5}"/>
+    <hyperlink ref="J5" r:id="rId3" xr:uid="{6F859BC4-A6BF-43EC-A7DD-B0D3FB7E2A5B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DA6FD2-F5FA-420E-85BD-83DA546D3326}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="6" width="8.6640625" style="1"/>
-    <col min="7" max="7" width="14.58203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="7" width="8.6640625" style="1"/>
+    <col min="8" max="8" width="14.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C1" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1247,21 +1293,24 @@
         <v>50000</v>
       </c>
       <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="22">
+        <v>4000</v>
+      </c>
+      <c r="F3" s="21">
+        <f>B3-(C3+D3+E3)</f>
+        <v>46000</v>
+      </c>
+      <c r="H3" s="35">
+        <f>50000 * 3-SUM(F3:F5)</f>
         <v>9000</v>
       </c>
-      <c r="D3" s="4">
-        <v>2000</v>
-      </c>
-      <c r="E3" s="21">
-        <f>B3-(C3+D3)</f>
-        <v>39000</v>
-      </c>
-      <c r="G3" s="32">
-        <f>50000 * 3-SUM(E3:E5)</f>
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1269,18 +1318,21 @@
         <v>50000</v>
       </c>
       <c r="C4" s="4">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="21">
-        <f t="shared" ref="E4:E5" si="0">B4-(C4+D4)</f>
-        <v>44000</v>
-      </c>
-      <c r="G4" s="33"/>
-    </row>
-    <row r="5" spans="1:7" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E4" s="22">
+        <v>3000</v>
+      </c>
+      <c r="F4" s="21">
+        <f t="shared" ref="F4:F5" si="0">B4-(C4+D4+E4)</f>
+        <v>47000</v>
+      </c>
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1288,21 +1340,24 @@
         <v>50000</v>
       </c>
       <c r="C5" s="4">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="22">
+        <v>2000</v>
+      </c>
+      <c r="F5" s="21">
         <f t="shared" si="0"/>
-        <v>44000</v>
-      </c>
-      <c r="G5" s="34"/>
+        <v>48000</v>
+      </c>
+      <c r="H5" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>